<commit_message>
Parallel processing implemented E
</commit_message>
<xml_diff>
--- a/deap/mj_projects/definitionbooks/nsga1_zdt1_Xbinary_Mbinary.xlsx
+++ b/deap/mj_projects/definitionbooks/nsga1_zdt1_Xbinary_Mbinary.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="2445" windowWidth="17490" windowHeight="6900" activeTab="2"/>
@@ -22,10 +22,10 @@
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
-    <author>Author</author>
+    <author>Autor</author>
   </authors>
   <commentList>
-    <comment ref="B4" authorId="0" shapeId="0">
+    <comment ref="B4" authorId="0">
       <text>
         <r>
           <rPr>
@@ -49,7 +49,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B5" authorId="0" shapeId="0">
+    <comment ref="B5" authorId="0">
       <text>
         <r>
           <rPr>
@@ -235,9 +235,6 @@
     <t>nsga2</t>
   </si>
   <si>
-    <t>evaluate</t>
-  </si>
-  <si>
     <t>select</t>
   </si>
   <si>
@@ -305,6 +302,9 @@
   </si>
   <si>
     <t>evaluate_pop</t>
+  </si>
+  <si>
+    <t>life_cycle</t>
   </si>
 </sst>
 </file>
@@ -381,7 +381,7 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -397,9 +397,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Larissa">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -437,9 +437,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Larissa">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -474,7 +474,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -509,7 +509,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Larissa">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -689,7 +689,7 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="23" bestFit="1" customWidth="1"/>
@@ -738,7 +738,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B6" t="s">
         <v>1</v>
@@ -759,7 +759,7 @@
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="27.42578125" customWidth="1"/>
   </cols>
@@ -769,10 +769,10 @@
         <v>53</v>
       </c>
       <c r="B1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C1" t="s">
         <v>63</v>
-      </c>
-      <c r="C1" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -783,7 +783,7 @@
         <v>40</v>
       </c>
       <c r="C2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -794,12 +794,12 @@
         <v>250</v>
       </c>
       <c r="C3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B4">
         <v>0.9</v>
@@ -810,7 +810,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -821,7 +821,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B6">
         <v>20</v>
@@ -832,7 +832,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B7" s="8">
         <v>3.3333333333333333E-2</v>
@@ -851,10 +851,10 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.7109375" bestFit="1" customWidth="1"/>
@@ -862,13 +862,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B1" t="s">
         <v>76</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>77</v>
-      </c>
-      <c r="C1" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -876,7 +876,7 @@
         <v>53</v>
       </c>
       <c r="B2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C2" t="s">
         <v>54</v>
@@ -884,24 +884,24 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>55</v>
+        <v>78</v>
       </c>
       <c r="B3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B4" t="s">
+        <v>57</v>
+      </c>
+      <c r="C4" t="s">
         <v>58</v>
-      </c>
-      <c r="C4" t="s">
-        <v>59</v>
       </c>
     </row>
   </sheetData>
@@ -918,7 +918,7 @@
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="22.140625" customWidth="1"/>
     <col min="2" max="2" width="19.28515625" customWidth="1"/>
@@ -927,35 +927,35 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>64</v>
+      </c>
+      <c r="B3" t="s">
         <v>65</v>
       </c>
-      <c r="B3" t="s">
-        <v>66</v>
-      </c>
       <c r="C3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
   </sheetData>
@@ -971,7 +971,7 @@
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.42578125" customWidth="1"/>
@@ -1520,7 +1520,7 @@
       <selection activeCell="A2" sqref="A2:XFD3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14" style="6" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.42578125" style="6" bestFit="1" customWidth="1"/>
@@ -1574,7 +1574,7 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="11.85546875" bestFit="1" customWidth="1"/>
   </cols>

</xml_diff>

<commit_message>
Update Crowding Distance Revisited; - Last Front NOT yet implemented - UFTourn complete - CrowdingDistanceRevised now operates on unique fitnesses
</commit_message>
<xml_diff>
--- a/deap/mj_projects/definitionbooks/nsga1_zdt1_Xbinary_Mbinary.xlsx
+++ b/deap/mj_projects/definitionbooks/nsga1_zdt1_Xbinary_Mbinary.xlsx
@@ -4,18 +4,19 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="17490" windowHeight="6900" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="17490" windowHeight="6900" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Project" sheetId="3" r:id="rId1"/>
     <sheet name="Parameters" sheetId="11" r:id="rId2"/>
     <sheet name="Algorithm" sheetId="9" r:id="rId3"/>
-    <sheet name="Operators" sheetId="7" r:id="rId4"/>
-    <sheet name="Range Variables" sheetId="1" r:id="rId5"/>
-    <sheet name="List Variables" sheetId="8" r:id="rId6"/>
-    <sheet name="Objectives" sheetId="4" r:id="rId7"/>
+    <sheet name="Tabelle1" sheetId="12" r:id="rId4"/>
+    <sheet name="Operators" sheetId="7" r:id="rId5"/>
+    <sheet name="Range Variables" sheetId="1" r:id="rId6"/>
+    <sheet name="List Variables" sheetId="8" r:id="rId7"/>
+    <sheet name="Objectives" sheetId="4" r:id="rId8"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
@@ -68,7 +69,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="80">
   <si>
     <t>Yes</t>
   </si>
@@ -244,9 +245,6 @@
     <t>tools</t>
   </si>
   <si>
-    <t>selNSGA2</t>
-  </si>
-  <si>
     <t>mj_evaluators</t>
   </si>
   <si>
@@ -305,6 +303,12 @@
   </si>
   <si>
     <t>life_cycle</t>
+  </si>
+  <si>
+    <t>selNSGA2revised</t>
+  </si>
+  <si>
+    <t>UFTournSelection</t>
   </si>
 </sst>
 </file>
@@ -738,7 +742,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B6" t="s">
         <v>1</v>
@@ -769,10 +773,10 @@
         <v>53</v>
       </c>
       <c r="B1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C1" t="s">
         <v>62</v>
-      </c>
-      <c r="C1" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -783,7 +787,7 @@
         <v>40</v>
       </c>
       <c r="C2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -794,12 +798,12 @@
         <v>250</v>
       </c>
       <c r="C3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B4">
         <v>0.9</v>
@@ -810,7 +814,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -821,7 +825,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B6">
         <v>20</v>
@@ -832,7 +836,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B7" s="8">
         <v>3.3333333333333333E-2</v>
@@ -850,25 +854,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B1" t="s">
         <v>75</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>76</v>
-      </c>
-      <c r="C1" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -876,7 +880,7 @@
         <v>53</v>
       </c>
       <c r="B2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C2" t="s">
         <v>54</v>
@@ -884,10 +888,10 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C3" t="s">
         <v>56</v>
@@ -901,7 +905,7 @@
         <v>57</v>
       </c>
       <c r="C4" t="s">
-        <v>58</v>
+        <v>78</v>
       </c>
     </row>
   </sheetData>
@@ -912,10 +916,36 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -933,29 +963,29 @@
         <v>57</v>
       </c>
       <c r="C1" t="s">
-        <v>66</v>
+        <v>79</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>63</v>
+      </c>
+      <c r="B3" t="s">
         <v>64</v>
       </c>
-      <c r="B3" t="s">
-        <v>65</v>
-      </c>
       <c r="C3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
   </sheetData>
@@ -963,7 +993,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E31"/>
   <sheetViews>
@@ -1512,7 +1542,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H1"/>
   <sheetViews>
@@ -1566,7 +1596,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B3"/>
   <sheetViews>

</xml_diff>